<commit_message>
add eluaat to source csv
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/materiaalklasse/materiaalklasse.xlsx
+++ b/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/materiaalklasse/materiaalklasse.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -466,7 +466,7 @@
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="E2" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dnapl|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eieren|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lnapl|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/melk|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/migratie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/puurproduct|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/schelpdieren|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dnapl|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eieren|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eluaat|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lnapl|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/melk|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/migratie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/puurproduct|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/schelpdieren|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
       </c>
       <c r="F2" t="str">
         <v>materiaalklasses</v>
@@ -1104,13 +1104,13 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eluaat</v>
       </c>
       <c r="B15" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C15" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.fruit</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.eluaat</v>
       </c>
       <c r="D15" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1119,19 +1119,19 @@
         <v>null</v>
       </c>
       <c r="F15" t="str">
-        <v>fruit</v>
+        <v>eluaat</v>
       </c>
       <c r="G15" t="str">
-        <v>Fruit</v>
+        <v>Eluaat</v>
       </c>
       <c r="H15" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="I15" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="J15" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="K15" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit</v>
       </c>
       <c r="B16" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C16" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.gftafval</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.fruit</v>
       </c>
       <c r="D16" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1169,10 +1169,10 @@
         <v>null</v>
       </c>
       <c r="F16" t="str">
-        <v>gftafval</v>
+        <v>fruit</v>
       </c>
       <c r="G16" t="str">
-        <v>GFT-afval</v>
+        <v>Fruit</v>
       </c>
       <c r="H16" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
@@ -1204,13 +1204,13 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval</v>
       </c>
       <c r="B17" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C17" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.groenten</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.gftafval</v>
       </c>
       <c r="D17" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1219,10 +1219,10 @@
         <v>null</v>
       </c>
       <c r="F17" t="str">
-        <v>groenten</v>
+        <v>gftafval</v>
       </c>
       <c r="G17" t="str">
-        <v>Groenten</v>
+        <v>GFT-afval</v>
       </c>
       <c r="H17" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
@@ -1254,13 +1254,13 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten</v>
       </c>
       <c r="B18" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C18" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.grondwater</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.groenten</v>
       </c>
       <c r="D18" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1269,19 +1269,19 @@
         <v>null</v>
       </c>
       <c r="F18" t="str">
-        <v>grondwater</v>
+        <v>groenten</v>
       </c>
       <c r="G18" t="str">
-        <v>Grondwater</v>
+        <v>Groenten</v>
       </c>
       <c r="H18" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="I18" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="J18" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="K18" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1304,13 +1304,13 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater</v>
       </c>
       <c r="B19" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C19" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.hardgesteente</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.grondwater</v>
       </c>
       <c r="D19" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1319,19 +1319,19 @@
         <v>null</v>
       </c>
       <c r="F19" t="str">
-        <v>hardgesteente</v>
+        <v>grondwater</v>
       </c>
       <c r="G19" t="str">
-        <v>Hard gesteente</v>
+        <v>Grondwater</v>
       </c>
       <c r="H19" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="I19" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="J19" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="K19" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1354,13 +1354,13 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente</v>
       </c>
       <c r="B20" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C20" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.koelwater</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.hardgesteente</v>
       </c>
       <c r="D20" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1369,19 +1369,19 @@
         <v>null</v>
       </c>
       <c r="F20" t="str">
-        <v>koelwater</v>
+        <v>hardgesteente</v>
       </c>
       <c r="G20" t="str">
-        <v>Koelwater</v>
+        <v>Hard gesteente</v>
       </c>
       <c r="H20" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="I20" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="J20" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="K20" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1404,13 +1404,13 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lnapl</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater</v>
       </c>
       <c r="B21" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C21" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.lnapl</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.koelwater</v>
       </c>
       <c r="D21" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1419,19 +1419,19 @@
         <v>null</v>
       </c>
       <c r="F21" t="str">
-        <v>lnapl</v>
+        <v>koelwater</v>
       </c>
       <c r="G21" t="str">
-        <v>Drijflaag (LNAPL)</v>
+        <v>Koelwater</v>
       </c>
       <c r="H21" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="I21" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="J21" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="K21" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1454,13 +1454,13 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lnapl</v>
       </c>
       <c r="B22" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C22" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.lucht</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.lnapl</v>
       </c>
       <c r="D22" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1469,28 +1469,28 @@
         <v>null</v>
       </c>
       <c r="F22" t="str">
-        <v>lucht</v>
+        <v>lnapl</v>
       </c>
       <c r="G22" t="str">
-        <v>Lucht</v>
+        <v>Drijflaag (LNAPL)</v>
       </c>
       <c r="H22" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
       </c>
       <c r="I22" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
       </c>
       <c r="J22" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
       </c>
       <c r="K22" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L22" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
+        <v>null</v>
       </c>
       <c r="M22" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
+        <v>null</v>
       </c>
       <c r="N22" t="str">
         <v>null</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/melk</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht</v>
       </c>
       <c r="B23" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C23" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.melk</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.lucht</v>
       </c>
       <c r="D23" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1519,28 +1519,28 @@
         <v>null</v>
       </c>
       <c r="F23" t="str">
-        <v>melk</v>
+        <v>lucht</v>
       </c>
       <c r="G23" t="str">
-        <v>Melk</v>
+        <v>Lucht</v>
       </c>
       <c r="H23" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
+        <v>null</v>
       </c>
       <c r="I23" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
+        <v>null</v>
       </c>
       <c r="J23" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
       </c>
       <c r="K23" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L23" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
       </c>
       <c r="M23" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
       </c>
       <c r="N23" t="str">
         <v>null</v>
@@ -1554,13 +1554,13 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/migratie</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/melk</v>
       </c>
       <c r="B24" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C24" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.migratie</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.melk</v>
       </c>
       <c r="D24" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1569,19 +1569,19 @@
         <v>null</v>
       </c>
       <c r="F24" t="str">
-        <v>migratie</v>
+        <v>melk</v>
       </c>
       <c r="G24" t="str">
-        <v>Migratie</v>
+        <v>Melk</v>
       </c>
       <c r="H24" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
       </c>
       <c r="I24" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
       </c>
       <c r="J24" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
       </c>
       <c r="K24" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1604,13 +1604,13 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/migratie</v>
       </c>
       <c r="B25" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C25" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.oppervlaktewater</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.migratie</v>
       </c>
       <c r="D25" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1619,19 +1619,19 @@
         <v>null</v>
       </c>
       <c r="F25" t="str">
-        <v>oppervlaktewater</v>
+        <v>migratie</v>
       </c>
       <c r="G25" t="str">
-        <v>Oppervlaktewater</v>
+        <v>Migratie</v>
       </c>
       <c r="H25" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>null</v>
       </c>
       <c r="I25" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>null</v>
       </c>
       <c r="J25" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>null</v>
       </c>
       <c r="K25" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1654,13 +1654,13 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater</v>
       </c>
       <c r="B26" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C26" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.plantaardigmateriaal</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.oppervlaktewater</v>
       </c>
       <c r="D26" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1669,28 +1669,28 @@
         <v>null</v>
       </c>
       <c r="F26" t="str">
-        <v>plantaardigmateriaal</v>
+        <v>oppervlaktewater</v>
       </c>
       <c r="G26" t="str">
-        <v>Plantaardig materiaal</v>
+        <v>Oppervlaktewater</v>
       </c>
       <c r="H26" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="I26" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="J26" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="K26" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L26" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt</v>
+        <v>null</v>
       </c>
       <c r="M26" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt</v>
+        <v>null</v>
       </c>
       <c r="N26" t="str">
         <v>null</v>
@@ -1704,13 +1704,13 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/puurproduct</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="B27" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C27" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.puurproduct</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.plantaardigmateriaal</v>
       </c>
       <c r="D27" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1719,28 +1719,28 @@
         <v>null</v>
       </c>
       <c r="F27" t="str">
-        <v>puurproduct</v>
+        <v>plantaardigmateriaal</v>
       </c>
       <c r="G27" t="str">
-        <v>Puur product</v>
+        <v>Plantaardig materiaal</v>
       </c>
       <c r="H27" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
+        <v>null</v>
       </c>
       <c r="I27" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
+        <v>null</v>
       </c>
       <c r="J27" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt</v>
       </c>
       <c r="K27" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L27" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt</v>
       </c>
       <c r="M27" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt</v>
       </c>
       <c r="N27" t="str">
         <v>null</v>
@@ -1754,13 +1754,13 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/puurproduct</v>
       </c>
       <c r="B28" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C28" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.regenwater</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.puurproduct</v>
       </c>
       <c r="D28" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1769,19 +1769,19 @@
         <v>null</v>
       </c>
       <c r="F28" t="str">
-        <v>regenwater</v>
+        <v>puurproduct</v>
       </c>
       <c r="G28" t="str">
-        <v>Regenwater</v>
+        <v>Puur product</v>
       </c>
       <c r="H28" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
       </c>
       <c r="I28" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
       </c>
       <c r="J28" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten</v>
       </c>
       <c r="K28" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1804,13 +1804,13 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/schelpdieren</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater</v>
       </c>
       <c r="B29" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C29" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.schelpdieren</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.regenwater</v>
       </c>
       <c r="D29" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1819,19 +1819,19 @@
         <v>null</v>
       </c>
       <c r="F29" t="str">
-        <v>schelpdieren</v>
+        <v>regenwater</v>
       </c>
       <c r="G29" t="str">
-        <v>Schelpdieren</v>
+        <v>Regenwater</v>
       </c>
       <c r="H29" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="I29" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="J29" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="K29" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/schelpdieren</v>
       </c>
       <c r="B30" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C30" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.sediment</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.schelpdieren</v>
       </c>
       <c r="D30" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1869,19 +1869,19 @@
         <v>null</v>
       </c>
       <c r="F30" t="str">
-        <v>sediment</v>
+        <v>schelpdieren</v>
       </c>
       <c r="G30" t="str">
-        <v>Sediment</v>
+        <v>Schelpdieren</v>
       </c>
       <c r="H30" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
       </c>
       <c r="I30" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
       </c>
       <c r="J30" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal</v>
       </c>
       <c r="K30" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1904,13 +1904,13 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment</v>
       </c>
       <c r="B31" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C31" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.strooisel</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.sediment</v>
       </c>
       <c r="D31" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1919,19 +1919,19 @@
         <v>null</v>
       </c>
       <c r="F31" t="str">
-        <v>strooisel</v>
+        <v>sediment</v>
       </c>
       <c r="G31" t="str">
-        <v>Strooisel</v>
+        <v>Sediment</v>
       </c>
       <c r="H31" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="I31" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="J31" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="K31" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1954,13 +1954,13 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel</v>
       </c>
       <c r="B32" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C32" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.vastdeelvdaarde</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.strooisel</v>
       </c>
       <c r="D32" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -1969,28 +1969,28 @@
         <v>null</v>
       </c>
       <c r="F32" t="str">
-        <v>vastdeelvdaarde</v>
+        <v>strooisel</v>
       </c>
       <c r="G32" t="str">
-        <v>Vaste deel van de aarde</v>
+        <v>Strooisel</v>
       </c>
       <c r="H32" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="I32" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="J32" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="K32" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L32" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem</v>
+        <v>null</v>
       </c>
       <c r="M32" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem</v>
+        <v>null</v>
       </c>
       <c r="N32" t="str">
         <v>null</v>
@@ -2004,13 +2004,13 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="B33" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C33" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.vilt</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.vastdeelvdaarde</v>
       </c>
       <c r="D33" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -2019,28 +2019,28 @@
         <v>null</v>
       </c>
       <c r="F33" t="str">
-        <v>vilt</v>
+        <v>vastdeelvdaarde</v>
       </c>
       <c r="G33" t="str">
-        <v>Vilt</v>
+        <v>Vaste deel van de aarde</v>
       </c>
       <c r="H33" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>null</v>
       </c>
       <c r="I33" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>null</v>
       </c>
       <c r="J33" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eluaat|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem</v>
       </c>
       <c r="K33" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L33" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eluaat|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem</v>
       </c>
       <c r="M33" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eluaat|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem</v>
       </c>
       <c r="N33" t="str">
         <v>null</v>
@@ -2054,13 +2054,13 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt</v>
       </c>
       <c r="B34" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C34" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.water</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.vilt</v>
       </c>
       <c r="D34" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -2069,28 +2069,28 @@
         <v>null</v>
       </c>
       <c r="F34" t="str">
-        <v>water</v>
+        <v>vilt</v>
       </c>
       <c r="G34" t="str">
-        <v>Water</v>
+        <v>Vilt</v>
       </c>
       <c r="H34" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="I34" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="J34" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal</v>
       </c>
       <c r="K34" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L34" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
+        <v>null</v>
       </c>
       <c r="M34" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
+        <v>null</v>
       </c>
       <c r="N34" t="str">
         <v>null</v>
@@ -2104,13 +2104,13 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="B35" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C35" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.waterbodem</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.water</v>
       </c>
       <c r="D35" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -2119,28 +2119,28 @@
         <v>null</v>
       </c>
       <c r="F35" t="str">
-        <v>waterbodem</v>
+        <v>water</v>
       </c>
       <c r="G35" t="str">
-        <v>Waterbodem</v>
+        <v>Water</v>
       </c>
       <c r="H35" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>null</v>
       </c>
       <c r="I35" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>null</v>
       </c>
       <c r="J35" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
       </c>
       <c r="K35" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L35" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
       </c>
       <c r="M35" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
       </c>
       <c r="N35" t="str">
         <v>null</v>
@@ -2154,13 +2154,13 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem</v>
       </c>
       <c r="B36" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C36" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.zeeschuim</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.waterbodem</v>
       </c>
       <c r="D36" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -2169,19 +2169,19 @@
         <v>null</v>
       </c>
       <c r="F36" t="str">
-        <v>zeeschuim</v>
+        <v>waterbodem</v>
       </c>
       <c r="G36" t="str">
-        <v>Zeeschuim</v>
+        <v>Waterbodem</v>
       </c>
       <c r="H36" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="I36" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="J36" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde</v>
       </c>
       <c r="K36" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -2204,43 +2204,43 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim</v>
+      </c>
+      <c r="B37" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+      </c>
+      <c r="C37" t="str">
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.zeeschuim</v>
+      </c>
+      <c r="D37" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
+      </c>
+      <c r="E37" t="str">
+        <v>null</v>
+      </c>
+      <c r="F37" t="str">
+        <v>zeeschuim</v>
+      </c>
+      <c r="G37" t="str">
+        <v>Zeeschuim</v>
+      </c>
+      <c r="H37" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
       </c>
-      <c r="B37" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
-      </c>
-      <c r="C37" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.zeewater</v>
-      </c>
-      <c r="D37" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
-      </c>
-      <c r="E37" t="str">
-        <v>null</v>
-      </c>
-      <c r="F37" t="str">
-        <v>zeewater</v>
-      </c>
-      <c r="G37" t="str">
-        <v>Zeewater</v>
-      </c>
-      <c r="H37" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
-      </c>
       <c r="I37" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
       </c>
       <c r="J37" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
       </c>
       <c r="K37" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L37" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim</v>
+        <v>null</v>
       </c>
       <c r="M37" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim</v>
+        <v>null</v>
       </c>
       <c r="N37" t="str">
         <v>null</v>
@@ -2254,13 +2254,13 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater</v>
       </c>
       <c r="B38" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C38" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.zwevendestof</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.zeewater</v>
       </c>
       <c r="D38" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
@@ -2269,28 +2269,28 @@
         <v>null</v>
       </c>
       <c r="F38" t="str">
-        <v>zwevendestof</v>
+        <v>zeewater</v>
       </c>
       <c r="G38" t="str">
-        <v>Zwevende stof</v>
+        <v>Zeewater</v>
       </c>
       <c r="H38" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="I38" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water</v>
       </c>
       <c r="J38" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim</v>
       </c>
       <c r="K38" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
       </c>
       <c r="L38" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim</v>
       </c>
       <c r="M38" t="str">
-        <v>null</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim</v>
       </c>
       <c r="N38" t="str">
         <v>null</v>
@@ -2304,57 +2304,107 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
       </c>
       <c r="B39" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+      </c>
+      <c r="C39" t="str">
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.materiaalklasse.zwevendestof</v>
+      </c>
+      <c r="D39" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
+      </c>
+      <c r="E39" t="str">
+        <v>null</v>
+      </c>
+      <c r="F39" t="str">
+        <v>zwevendestof</v>
+      </c>
+      <c r="G39" t="str">
+        <v>Zwevende stof</v>
+      </c>
+      <c r="H39" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht</v>
+      </c>
+      <c r="I39" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht</v>
+      </c>
+      <c r="J39" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht</v>
+      </c>
+      <c r="K39" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
+      </c>
+      <c r="L39" t="str">
+        <v>null</v>
+      </c>
+      <c r="M39" t="str">
+        <v>null</v>
+      </c>
+      <c r="N39" t="str">
+        <v>null</v>
+      </c>
+      <c r="O39" t="str">
+        <v>null</v>
+      </c>
+      <c r="P39" t="str">
+        <v>null</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/materiaalklasse</v>
+      </c>
+      <c r="B40" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C40" t="str">
         <v>be.vlaanderen.bodemenondergrond.data.id.conceptscheme.materiaalklasse</v>
       </c>
-      <c r="D39" t="str">
-        <v>null</v>
-      </c>
-      <c r="E39" t="str">
-        <v>null</v>
-      </c>
-      <c r="F39" t="str">
+      <c r="D40" t="str">
+        <v>null</v>
+      </c>
+      <c r="E40" t="str">
+        <v>null</v>
+      </c>
+      <c r="F40" t="str">
         <v>materiaalklasse</v>
       </c>
-      <c r="G39" t="str">
+      <c r="G40" t="str">
         <v>Codelijst materiaalklasse.</v>
       </c>
-      <c r="H39" t="str">
-        <v>null</v>
-      </c>
-      <c r="I39" t="str">
-        <v>null</v>
-      </c>
-      <c r="J39" t="str">
-        <v>null</v>
-      </c>
-      <c r="K39" t="str">
-        <v>null</v>
-      </c>
-      <c r="L39" t="str">
-        <v>null</v>
-      </c>
-      <c r="M39" t="str">
-        <v>null</v>
-      </c>
-      <c r="N39" t="str">
+      <c r="H40" t="str">
+        <v>null</v>
+      </c>
+      <c r="I40" t="str">
+        <v>null</v>
+      </c>
+      <c r="J40" t="str">
+        <v>null</v>
+      </c>
+      <c r="K40" t="str">
+        <v>null</v>
+      </c>
+      <c r="L40" t="str">
+        <v>null</v>
+      </c>
+      <c r="M40" t="str">
+        <v>null</v>
+      </c>
+      <c r="N40" t="str">
         <v>Aard van de Bemonstering.</v>
       </c>
-      <c r="O39" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dnapl|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eieren|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lnapl|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/melk|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/migratie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/puurproduct|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/schelpdieren|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
-      </c>
-      <c r="P39" t="str">
+      <c r="O40" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/afvalwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/antropogeneobjecten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bemalingswater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemlucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/bodemvocht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/depositie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dierlijkmateriaal|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/dnapl|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/drinkwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/effluent|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eieren|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/eluaat|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/fruit|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/gftafval|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/groenten|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/grondwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/hardgesteente|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/koelwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lnapl|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/lucht|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/melk|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/migratie|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/oppervlaktewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/plantaardigmateriaal|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/puurproduct|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/regenwater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/schelpdieren|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/sediment|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/strooisel|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vastdeelvdaarde|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/vilt|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/water|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/waterbodem|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeeschuim|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zeewater|https://data.bodemenondergrond.vlaanderen.be/id/concept/materiaalklasse/zwevendestof</v>
+      </c>
+      <c r="P40" t="str">
         <v>Aard van de Bemonstering.</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P40"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>